<commit_message>
value tier 1 and tier 2 jointly
</commit_message>
<xml_diff>
--- a/model/RunControl.xlsx
+++ b/model/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064FC27C-88C9-4DAF-AE9B-8325241AED56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F343AB71-9EF7-44DF-A8FD-3BC38EBF0F5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params_sim" sheetId="22" r:id="rId1"/>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="1" shapeId="0" xr:uid="{1E17415D-3C00-4D50-B13B-6BE374701D46}">
+    <comment ref="I4" authorId="1" shapeId="0" xr:uid="{1E17415D-3C00-4D50-B13B-6BE374701D46}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -78,7 +78,7 @@
     See tab "Note1" for explanations of the combinations of parameters "use_baselineUAAL" and "newBasisPolicyChg"</t>
       </text>
     </comment>
-    <comment ref="W4" authorId="2" shapeId="0" xr:uid="{2BAAEFE0-093F-4A47-AC11-22B6E01FEF48}">
+    <comment ref="X4" authorId="2" shapeId="0" xr:uid="{2BAAEFE0-093F-4A47-AC11-22B6E01FEF48}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -86,7 +86,7 @@
     COLA when risk-sharing is not triggered</t>
       </text>
     </comment>
-    <comment ref="AC4" authorId="3" shapeId="0" xr:uid="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
+    <comment ref="AD4" authorId="3" shapeId="0" xr:uid="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -94,7 +94,7 @@
     The esclator is calibrated from 2.75% to 3.5% to match the 2018 SC</t>
       </text>
     </comment>
-    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{568404F5-400A-46EF-8AA1-93D4C44E460E}">
+    <comment ref="AH4" authorId="0" shapeId="0" xr:uid="{568404F5-400A-46EF-8AA1-93D4C44E460E}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ4" authorId="0" shapeId="0" xr:uid="{148CF5FB-6519-420B-97E2-DCE9E3F8AE4C}">
+    <comment ref="AR4" authorId="0" shapeId="0" xr:uid="{148CF5FB-6519-420B-97E2-DCE9E3F8AE4C}">
       <text>
         <r>
           <rPr>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="316">
   <si>
     <t>nsim</t>
   </si>
@@ -1489,6 +1489,27 @@
   </si>
   <si>
     <t>sal_pre2019</t>
+  </si>
+  <si>
+    <t>Dev_pf.t2</t>
+  </si>
+  <si>
+    <t>"pf.t2"</t>
+  </si>
+  <si>
+    <t>Dev_pf</t>
+  </si>
+  <si>
+    <t>val_tierName</t>
+  </si>
+  <si>
+    <t>pf.t1</t>
+  </si>
+  <si>
+    <t>"pf.t1","pf.t2"</t>
+  </si>
+  <si>
+    <t>pf.t2</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1844,7 @@
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2109,6 +2130,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="17" fillId="14" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2430,13 +2460,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H4" dT="2020-11-29T15:06:08.38" personId="{00000000-0000-0000-0000-000000000000}" id="{1E17415D-3C00-4D50-B13B-6BE374701D46}">
+  <threadedComment ref="I4" dT="2020-11-29T15:06:08.38" personId="{00000000-0000-0000-0000-000000000000}" id="{1E17415D-3C00-4D50-B13B-6BE374701D46}">
     <text>See tab "Note1" for explanations of the combinations of parameters "use_baselineUAAL" and "newBasisPolicyChg"</text>
   </threadedComment>
-  <threadedComment ref="W4" dT="2021-03-13T00:37:48.89" personId="{00000000-0000-0000-0000-000000000000}" id="{2BAAEFE0-093F-4A47-AC11-22B6E01FEF48}">
+  <threadedComment ref="X4" dT="2021-03-13T00:37:48.89" personId="{00000000-0000-0000-0000-000000000000}" id="{2BAAEFE0-093F-4A47-AC11-22B6E01FEF48}">
     <text>COLA when risk-sharing is not triggered</text>
   </threadedComment>
-  <threadedComment ref="AC4" dT="2020-12-06T12:17:58.66" personId="{00000000-0000-0000-0000-000000000000}" id="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
+  <threadedComment ref="AD4" dT="2020-12-06T12:17:58.66" personId="{00000000-0000-0000-0000-000000000000}" id="{8515E407-C037-4E97-A4C6-62FC0108B1A6}">
     <text>The esclator is calibrated from 2.75% to 3.5% to match the 2018 SC</text>
   </threadedComment>
 </ThreadedComments>
@@ -2471,64 +2501,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D014B46A-D012-4D18-AEAB-1D829080B2CE}">
-  <dimension ref="A2:BC18"/>
+  <dimension ref="A2:BD18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="I5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K33" sqref="K33"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" customWidth="1"/>
-    <col min="19" max="21" width="12.5703125" customWidth="1"/>
-    <col min="22" max="25" width="17.42578125" customWidth="1"/>
-    <col min="26" max="26" width="15.5703125" customWidth="1"/>
-    <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.85546875" customWidth="1"/>
-    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.7109375" customWidth="1"/>
-    <col min="35" max="35" width="12.5703125" customWidth="1"/>
-    <col min="36" max="36" width="14.85546875" customWidth="1"/>
-    <col min="42" max="42" width="17.42578125" customWidth="1"/>
-    <col min="43" max="43" width="13.7109375" customWidth="1"/>
-    <col min="44" max="44" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="12.42578125" customWidth="1"/>
-    <col min="48" max="48" width="23" customWidth="1"/>
-    <col min="49" max="49" width="16.5703125" customWidth="1"/>
-    <col min="50" max="50" width="12" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.28515625" customWidth="1"/>
-    <col min="54" max="54" width="11.42578125" customWidth="1"/>
-    <col min="55" max="55" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="18" width="12.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="26" width="17.42578125" customWidth="1"/>
+    <col min="27" max="27" width="15.5703125" customWidth="1"/>
+    <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" customWidth="1"/>
+    <col min="36" max="36" width="12.5703125" customWidth="1"/>
+    <col min="37" max="37" width="14.85546875" customWidth="1"/>
+    <col min="43" max="43" width="17.42578125" customWidth="1"/>
+    <col min="44" max="44" width="13.7109375" customWidth="1"/>
+    <col min="45" max="45" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="12.42578125" customWidth="1"/>
+    <col min="49" max="49" width="23" customWidth="1"/>
+    <col min="50" max="50" width="16.5703125" customWidth="1"/>
+    <col min="51" max="51" width="12" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.28515625" customWidth="1"/>
+    <col min="55" max="55" width="11.42578125" customWidth="1"/>
+    <col min="56" max="56" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:55">
-      <c r="AR2" s="23"/>
+    <row r="2" spans="1:56">
       <c r="AS2" s="23"/>
-    </row>
-    <row r="3" spans="1:55" s="21" customFormat="1" ht="18.75">
+      <c r="AT2" s="23"/>
+    </row>
+    <row r="3" spans="1:56" s="21" customFormat="1" ht="18.75">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -2537,16 +2568,16 @@
         <v>73</v>
       </c>
       <c r="F3" s="19"/>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="44"/>
       <c r="I3" s="44"/>
       <c r="J3" s="44"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="44"/>
+      <c r="L3" s="59" t="s">
         <v>260</v>
       </c>
-      <c r="L3" s="59"/>
       <c r="M3" s="59"/>
       <c r="N3" s="59"/>
       <c r="O3" s="59"/>
@@ -2560,48 +2591,49 @@
       <c r="W3" s="59"/>
       <c r="X3" s="59"/>
       <c r="Y3" s="59"/>
-      <c r="Z3" s="16" t="s">
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AA3" s="16"/>
       <c r="AB3" s="16"/>
       <c r="AC3" s="16"/>
-      <c r="AD3" s="17" t="s">
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AE3" s="17"/>
       <c r="AF3" s="17"/>
       <c r="AG3" s="17"/>
       <c r="AH3" s="17"/>
-      <c r="AI3" s="19" t="s">
+      <c r="AI3" s="17"/>
+      <c r="AJ3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="AJ3" s="19"/>
       <c r="AK3" s="19"/>
       <c r="AL3" s="19"/>
       <c r="AM3" s="19"/>
       <c r="AN3" s="19"/>
       <c r="AO3" s="19"/>
-      <c r="AP3" s="15" t="s">
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AQ3" s="15"/>
       <c r="AR3" s="15"/>
       <c r="AS3" s="15"/>
       <c r="AT3" s="15"/>
       <c r="AU3" s="15"/>
       <c r="AV3" s="15"/>
-      <c r="AW3" s="20" t="s">
+      <c r="AW3" s="15"/>
+      <c r="AX3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AX3" s="20"/>
       <c r="AY3" s="20"/>
       <c r="AZ3" s="20"/>
       <c r="BA3" s="20"/>
       <c r="BB3" s="20"/>
       <c r="BC3" s="20"/>
-    </row>
-    <row r="4" spans="1:55" s="1" customFormat="1">
+      <c r="BD3" s="20"/>
+    </row>
+    <row r="4" spans="1:56" s="1" customFormat="1">
       <c r="A4" s="11" t="s">
         <v>75</v>
       </c>
@@ -2618,162 +2650,165 @@
         <v>70</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="H4" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="I4" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="J4" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="K4" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="L4" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="L4" s="62" t="s">
+      <c r="M4" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="N4" s="60" t="s">
         <v>246</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="O4" s="60" t="s">
         <v>231</v>
       </c>
-      <c r="O4" s="60" t="s">
+      <c r="P4" s="60" t="s">
         <v>232</v>
       </c>
-      <c r="P4" s="60" t="s">
+      <c r="Q4" s="60" t="s">
         <v>233</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="R4" s="60" t="s">
         <v>234</v>
       </c>
-      <c r="R4" s="60" t="s">
+      <c r="S4" s="60" t="s">
         <v>253</v>
       </c>
-      <c r="S4" s="60" t="s">
+      <c r="T4" s="60" t="s">
         <v>242</v>
       </c>
-      <c r="T4" s="60" t="s">
+      <c r="U4" s="60" t="s">
         <v>243</v>
       </c>
-      <c r="U4" s="60" t="s">
+      <c r="V4" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="V4" s="60" t="s">
+      <c r="W4" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="W4" s="60" t="s">
+      <c r="X4" s="60" t="s">
         <v>255</v>
       </c>
-      <c r="X4" s="60" t="s">
+      <c r="Y4" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="Y4" s="60" t="s">
+      <c r="Z4" s="60" t="s">
         <v>241</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="AA4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AA4" s="10" t="s">
+      <c r="AB4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="10" t="s">
+      <c r="AC4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="10" t="s">
+      <c r="AD4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AD4" s="9" t="s">
+      <c r="AE4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AE4" s="9" t="s">
+      <c r="AF4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AF4" s="9" t="s">
+      <c r="AG4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AG4" s="9" t="s">
+      <c r="AH4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AH4" s="9" t="s">
+      <c r="AI4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AI4" s="7" t="s">
+      <c r="AJ4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AJ4" s="7" t="s">
+      <c r="AK4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AK4" s="7" t="s">
+      <c r="AL4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AL4" s="7" t="s">
+      <c r="AM4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AM4" s="7" t="s">
+      <c r="AN4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="7" t="s">
+      <c r="AO4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AO4" s="7" t="s">
+      <c r="AP4" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="AP4" s="8" t="s">
+      <c r="AQ4" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AQ4" s="8" t="s">
+      <c r="AR4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AR4" s="8" t="s">
+      <c r="AS4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AS4" s="8" t="s">
+      <c r="AT4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AT4" s="8" t="s">
+      <c r="AU4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AU4" s="8" t="s">
+      <c r="AV4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AV4" s="8" t="s">
+      <c r="AW4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AW4" s="12" t="s">
+      <c r="AX4" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AX4" s="12" t="s">
+      <c r="AY4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AY4" s="12" t="s">
+      <c r="AZ4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AZ4" s="12" t="s">
+      <c r="BA4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="BA4" s="12" t="s">
+      <c r="BB4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="BB4" s="12" t="s">
+      <c r="BC4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="BC4" s="63" t="s">
+      <c r="BD4" s="63" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:56">
       <c r="A5" t="s">
         <v>259</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -2781,241 +2816,673 @@
       <c r="E5" t="s">
         <v>259</v>
       </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
         <v>72</v>
       </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
         <v>247</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>245</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.08</v>
       </c>
-      <c r="N5" s="61">
+      <c r="O5" s="61">
         <v>0.125</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.09</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.58140000000000003</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.41860000000000003</v>
       </c>
-      <c r="S5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5">
+      <c r="T5" t="b">
         <v>0</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>1.9099999999999999E-2</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="s">
         <v>230</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>35</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>20</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>5</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>999</v>
       </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="s">
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="s">
         <v>257</v>
       </c>
-      <c r="AH5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI5" t="s">
+      <c r="AI5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>105</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>20</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="AL5">
+      <c r="AM5">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AM5" s="3">
+      <c r="AN5" s="3">
         <v>0.12</v>
       </c>
-      <c r="AN5" s="5">
+      <c r="AO5" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AO5" s="38">
+      <c r="AP5" s="38">
         <v>123</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>31</v>
       </c>
       <c r="AQ5" t="s">
         <v>31</v>
       </c>
-      <c r="AR5" s="23">
-        <v>0.88300000000000001</v>
+      <c r="AR5" t="s">
+        <v>31</v>
       </c>
       <c r="AS5" s="23">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="AV5" s="43">
-        <v>0</v>
-      </c>
-      <c r="AW5" t="b">
-        <v>1</v>
+        <v>0.7</v>
+      </c>
+      <c r="AT5" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="AW5" s="43">
+        <v>0</v>
       </c>
       <c r="AX5" t="b">
         <v>1</v>
       </c>
       <c r="AY5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ5">
-        <v>0</v>
-      </c>
-      <c r="BA5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ5" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA5">
+        <v>0</v>
+      </c>
+      <c r="BB5" t="s">
         <v>3</v>
       </c>
-      <c r="BB5" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC5" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:55">
-      <c r="N6" s="61"/>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="5"/>
-      <c r="AO6" s="38"/>
-      <c r="AR6" s="23"/>
-      <c r="AS6" s="23"/>
-      <c r="AV6" s="43"/>
-      <c r="BC6" s="22"/>
-    </row>
-    <row r="7" spans="1:55">
-      <c r="N7" s="61"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="5"/>
-      <c r="AO7" s="38"/>
-      <c r="AR7" s="23"/>
+      <c r="BC5" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD5" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56">
+      <c r="A6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>309</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>247</v>
+      </c>
+      <c r="M6" t="s">
+        <v>245</v>
+      </c>
+      <c r="N6">
+        <v>0.08</v>
+      </c>
+      <c r="O6" s="61">
+        <v>0.125</v>
+      </c>
+      <c r="P6">
+        <v>0.09</v>
+      </c>
+      <c r="Q6">
+        <v>0.58140000000000003</v>
+      </c>
+      <c r="R6">
+        <v>0.41860000000000003</v>
+      </c>
+      <c r="T6" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="Y6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC6">
+        <v>20</v>
+      </c>
+      <c r="AD6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE6">
+        <v>5</v>
+      </c>
+      <c r="AF6">
+        <v>999</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL6">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="AM6">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AN6" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AP6" s="38">
+        <v>123</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS6" s="23">
+        <v>1</v>
+      </c>
+      <c r="AT6" s="23">
+        <v>1</v>
+      </c>
+      <c r="AW6" s="43">
+        <v>0</v>
+      </c>
+      <c r="AX6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ6" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC6" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD6" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56">
+      <c r="O7" s="61"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="38"/>
       <c r="AS7" s="23"/>
-      <c r="AV7" s="43"/>
-      <c r="BC7" s="22"/>
-    </row>
-    <row r="8" spans="1:55">
-      <c r="N8" s="61"/>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="5"/>
-      <c r="AO8" s="38"/>
-      <c r="AR8" s="23"/>
-      <c r="AS8" s="23"/>
-      <c r="AV8" s="43"/>
-      <c r="BC8" s="22"/>
-    </row>
-    <row r="9" spans="1:55">
-      <c r="N9" s="61"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="5"/>
-      <c r="AO9" s="38"/>
-      <c r="AR9" s="23"/>
-      <c r="AS9" s="23"/>
-      <c r="AV9" s="43"/>
-      <c r="BC9" s="22"/>
-    </row>
-    <row r="10" spans="1:55">
-      <c r="N10" s="61"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="5"/>
-      <c r="AO10" s="38"/>
-      <c r="AR10" s="23"/>
+      <c r="AT7" s="23"/>
+      <c r="AW7" s="43"/>
+      <c r="BD7" s="22"/>
+    </row>
+    <row r="8" spans="1:56">
+      <c r="A8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" t="s">
+        <v>313</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>247</v>
+      </c>
+      <c r="M8" t="s">
+        <v>245</v>
+      </c>
+      <c r="N8">
+        <v>0.08</v>
+      </c>
+      <c r="O8" s="61">
+        <v>0.125</v>
+      </c>
+      <c r="P8">
+        <v>0.09</v>
+      </c>
+      <c r="Q8">
+        <v>0.58140000000000003</v>
+      </c>
+      <c r="R8">
+        <v>0.41860000000000003</v>
+      </c>
+      <c r="T8" t="b">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="Y8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC8">
+        <v>20</v>
+      </c>
+      <c r="AD8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE8">
+        <v>5</v>
+      </c>
+      <c r="AF8">
+        <v>999</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL8">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="AM8">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AN8" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AO8" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AP8" s="38">
+        <v>123</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS8" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="AT8" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="AW8" s="43">
+        <v>0</v>
+      </c>
+      <c r="AX8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC8" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD8" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56">
+      <c r="A9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F9" t="s">
+        <v>315</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>247</v>
+      </c>
+      <c r="M9" t="s">
+        <v>245</v>
+      </c>
+      <c r="N9">
+        <v>0.08</v>
+      </c>
+      <c r="O9" s="61">
+        <v>0.125</v>
+      </c>
+      <c r="P9">
+        <v>0.09</v>
+      </c>
+      <c r="Q9">
+        <v>0.58140000000000003</v>
+      </c>
+      <c r="R9">
+        <v>0.41860000000000003</v>
+      </c>
+      <c r="T9" t="b">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="Y9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC9">
+        <v>20</v>
+      </c>
+      <c r="AD9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AE9">
+        <v>5</v>
+      </c>
+      <c r="AF9">
+        <v>999</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL9">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="AM9">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AO9" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AP9" s="38">
+        <v>123</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS9" s="23">
+        <v>1</v>
+      </c>
+      <c r="AT9" s="23">
+        <v>1</v>
+      </c>
+      <c r="AW9" s="43">
+        <v>0</v>
+      </c>
+      <c r="AX9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC9" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD9" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56">
+      <c r="O10" s="61"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="38"/>
       <c r="AS10" s="23"/>
-      <c r="AV10" s="43"/>
-      <c r="BC10" s="22"/>
-    </row>
-    <row r="11" spans="1:55">
-      <c r="N11" s="61"/>
-      <c r="AM11" s="3"/>
-      <c r="AN11" s="5"/>
-      <c r="AO11" s="38"/>
-      <c r="AR11" s="23"/>
+      <c r="AT10" s="23"/>
+      <c r="AW10" s="43"/>
+      <c r="BD10" s="22"/>
+    </row>
+    <row r="11" spans="1:56">
+      <c r="O11" s="61"/>
+      <c r="AN11" s="3"/>
+      <c r="AO11" s="5"/>
+      <c r="AP11" s="38"/>
       <c r="AS11" s="23"/>
-      <c r="AV11" s="43"/>
-      <c r="BC11" s="22"/>
-    </row>
-    <row r="12" spans="1:55">
-      <c r="N12" s="61"/>
-      <c r="AM12" s="3"/>
-      <c r="AN12" s="5"/>
-      <c r="AO12" s="38"/>
-      <c r="AR12" s="23"/>
+      <c r="AT11" s="23"/>
+      <c r="AW11" s="43"/>
+      <c r="BD11" s="22"/>
+    </row>
+    <row r="12" spans="1:56">
+      <c r="O12" s="61"/>
+      <c r="AN12" s="3"/>
+      <c r="AO12" s="5"/>
+      <c r="AP12" s="38"/>
       <c r="AS12" s="23"/>
-      <c r="AV12" s="43"/>
-      <c r="BC12" s="22"/>
-    </row>
-    <row r="13" spans="1:55">
-      <c r="N13" s="61"/>
-      <c r="AM13" s="3"/>
-      <c r="AN13" s="5"/>
-      <c r="AO13" s="38"/>
-      <c r="AR13" s="23"/>
+      <c r="AT12" s="23"/>
+      <c r="AW12" s="43"/>
+      <c r="BD12" s="22"/>
+    </row>
+    <row r="13" spans="1:56">
+      <c r="O13" s="61"/>
+      <c r="AN13" s="3"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="38"/>
       <c r="AS13" s="23"/>
-      <c r="AV13" s="43"/>
-      <c r="BC13" s="22"/>
-    </row>
-    <row r="14" spans="1:55">
-      <c r="N14" s="61"/>
-      <c r="AM14" s="3"/>
-      <c r="AN14" s="5"/>
-      <c r="AO14" s="38"/>
-      <c r="AR14" s="23"/>
+      <c r="AT13" s="23"/>
+      <c r="AW13" s="43"/>
+      <c r="BD13" s="22"/>
+    </row>
+    <row r="14" spans="1:56">
+      <c r="O14" s="61"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="5"/>
+      <c r="AP14" s="38"/>
       <c r="AS14" s="23"/>
-      <c r="AV14" s="43"/>
-      <c r="BC14" s="22"/>
-    </row>
-    <row r="15" spans="1:55">
+      <c r="AT14" s="23"/>
+      <c r="AW14" s="43"/>
+      <c r="BD14" s="22"/>
+    </row>
+    <row r="15" spans="1:56">
       <c r="B15" s="55" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:55">
+    <row r="16" spans="1:56">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -3031,152 +3498,152 @@
       <c r="E16" t="s">
         <v>229</v>
       </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
         <v>72</v>
       </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
         <v>236</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>237</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>0.06</v>
       </c>
-      <c r="N16" s="61">
+      <c r="O16" s="61">
         <v>0.125</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.09</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>0.58140000000000003</v>
-      </c>
-      <c r="Q16">
-        <v>0.41860000000000003</v>
       </c>
       <c r="R16">
         <v>0.41860000000000003</v>
       </c>
-      <c r="S16" t="b">
-        <v>0</v>
-      </c>
-      <c r="T16">
+      <c r="S16">
+        <v>0.41860000000000003</v>
+      </c>
+      <c r="T16" t="b">
         <v>0</v>
       </c>
       <c r="U16">
         <v>0</v>
       </c>
       <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
         <v>1.9099999999999999E-2</v>
-      </c>
-      <c r="W16">
-        <v>2.5000000000000001E-2</v>
       </c>
       <c r="X16">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="s">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="s">
         <v>230</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
         <v>35</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>20</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>2.75E-2</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>3</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>999</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
-      <c r="AG16" t="s">
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16" t="s">
         <v>257</v>
       </c>
-      <c r="AH16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI16" t="s">
+      <c r="AI16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ16" t="s">
         <v>105</v>
       </c>
-      <c r="AJ16" t="s">
+      <c r="AK16" t="s">
         <v>20</v>
       </c>
-      <c r="AK16">
+      <c r="AL16">
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AM16" s="3">
+      <c r="AN16" s="3">
         <v>0.12</v>
       </c>
-      <c r="AN16" s="5">
+      <c r="AO16" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AO16" s="38">
+      <c r="AP16" s="38">
         <v>123</v>
-      </c>
-      <c r="AP16" t="s">
-        <v>31</v>
       </c>
       <c r="AQ16" t="s">
         <v>31</v>
       </c>
-      <c r="AR16" s="23">
+      <c r="AR16" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS16" s="23">
         <v>0.88300000000000001</v>
       </c>
-      <c r="AS16" s="23">
+      <c r="AT16" s="23">
         <v>0.89900000000000002</v>
       </c>
-      <c r="AV16" s="43">
-        <v>0</v>
-      </c>
-      <c r="AW16" t="b">
-        <v>1</v>
+      <c r="AW16" s="43">
+        <v>0</v>
       </c>
       <c r="AX16" t="b">
         <v>1</v>
       </c>
       <c r="AY16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ16">
-        <v>0</v>
-      </c>
-      <c r="BA16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ16" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA16">
+        <v>0</v>
+      </c>
+      <c r="BB16" t="s">
         <v>3</v>
       </c>
-      <c r="BB16" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC16" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:55">
+      <c r="BC16" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD16" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56">
       <c r="A17" t="s">
         <v>249</v>
       </c>
@@ -3192,152 +3659,152 @@
       <c r="E17" t="s">
         <v>229</v>
       </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
         <v>72</v>
       </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
         <v>236</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>245</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>0.06</v>
       </c>
-      <c r="N17" s="61">
+      <c r="O17" s="61">
         <v>0.125</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>0.09</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>0.58140000000000003</v>
-      </c>
-      <c r="Q17">
-        <v>0.41860000000000003</v>
       </c>
       <c r="R17">
         <v>0.41860000000000003</v>
       </c>
-      <c r="S17" t="b">
-        <v>0</v>
-      </c>
-      <c r="T17">
+      <c r="S17">
+        <v>0.41860000000000003</v>
+      </c>
+      <c r="T17" t="b">
         <v>0</v>
       </c>
       <c r="U17">
         <v>0</v>
       </c>
       <c r="V17">
-        <v>1.9099999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="W17">
         <v>1.9099999999999999E-2</v>
       </c>
       <c r="X17">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="Y17">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17" t="s">
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="s">
         <v>230</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AB17" t="s">
         <v>35</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>20</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>2.75E-2</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>3</v>
       </c>
-      <c r="AE17">
+      <c r="AF17">
         <v>999</v>
       </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
-      <c r="AG17" t="s">
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17" t="s">
         <v>257</v>
       </c>
-      <c r="AH17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI17" t="s">
+      <c r="AI17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ17" t="s">
         <v>105</v>
       </c>
-      <c r="AJ17" t="s">
+      <c r="AK17" t="s">
         <v>20</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AM17" s="3">
+      <c r="AN17" s="3">
         <v>0.12</v>
       </c>
-      <c r="AN17" s="5">
+      <c r="AO17" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AO17" s="38">
+      <c r="AP17" s="38">
         <v>123</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>31</v>
       </c>
       <c r="AQ17" t="s">
         <v>31</v>
       </c>
-      <c r="AR17" s="23">
+      <c r="AR17" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS17" s="23">
         <v>0.88300000000000001</v>
       </c>
-      <c r="AS17" s="23">
+      <c r="AT17" s="23">
         <v>0.89900000000000002</v>
       </c>
-      <c r="AV17" s="43">
-        <v>0</v>
-      </c>
-      <c r="AW17" t="b">
-        <v>1</v>
+      <c r="AW17" s="43">
+        <v>0</v>
       </c>
       <c r="AX17" t="b">
         <v>1</v>
       </c>
       <c r="AY17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ17">
-        <v>0</v>
-      </c>
-      <c r="BA17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ17" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA17">
+        <v>0</v>
+      </c>
+      <c r="BB17" t="s">
         <v>3</v>
       </c>
-      <c r="BB17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC17" s="22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:55">
+      <c r="BC17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD17" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:56">
       <c r="A18" t="s">
         <v>254</v>
       </c>
@@ -3353,161 +3820,161 @@
       <c r="E18" t="s">
         <v>229</v>
       </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>72</v>
       </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
         <v>252</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>245</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>0.06</v>
       </c>
-      <c r="N18" s="61">
+      <c r="O18" s="61">
         <v>0.125</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>0.09</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>0.58140000000000003</v>
-      </c>
-      <c r="Q18">
-        <v>0.41860000000000003</v>
       </c>
       <c r="R18">
         <v>0.41860000000000003</v>
       </c>
-      <c r="S18" t="b">
-        <v>0</v>
-      </c>
-      <c r="T18">
+      <c r="S18">
+        <v>0.41860000000000003</v>
+      </c>
+      <c r="T18" t="b">
         <v>0</v>
       </c>
       <c r="U18">
         <v>0</v>
       </c>
       <c r="V18">
-        <v>1.9099999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="W18">
         <v>1.9099999999999999E-2</v>
       </c>
       <c r="X18">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="Y18">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="s">
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="s">
         <v>230</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AB18" t="s">
         <v>35</v>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <v>20</v>
       </c>
-      <c r="AC18">
+      <c r="AD18">
         <v>2.75E-2</v>
       </c>
-      <c r="AD18">
+      <c r="AE18">
         <v>3</v>
       </c>
-      <c r="AE18">
+      <c r="AF18">
         <v>999</v>
       </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
-      <c r="AG18" t="s">
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18" t="s">
         <v>257</v>
       </c>
-      <c r="AH18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI18" t="s">
+      <c r="AI18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ18" t="s">
         <v>105</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AK18" t="s">
         <v>20</v>
       </c>
-      <c r="AK18">
+      <c r="AL18">
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="AL18">
+      <c r="AM18">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AM18" s="3">
+      <c r="AN18" s="3">
         <v>0.12</v>
       </c>
-      <c r="AN18" s="5">
+      <c r="AO18" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AO18" s="38">
+      <c r="AP18" s="38">
         <v>123</v>
-      </c>
-      <c r="AP18" t="s">
-        <v>31</v>
       </c>
       <c r="AQ18" t="s">
         <v>31</v>
       </c>
-      <c r="AR18" s="23">
+      <c r="AR18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS18" s="23">
         <v>0.88300000000000001</v>
       </c>
-      <c r="AS18" s="23">
+      <c r="AT18" s="23">
         <v>0.89900000000000002</v>
       </c>
-      <c r="AV18" s="43">
-        <v>0</v>
-      </c>
-      <c r="AW18" t="b">
-        <v>1</v>
+      <c r="AW18" s="43">
+        <v>0</v>
       </c>
       <c r="AX18" t="b">
         <v>1</v>
       </c>
       <c r="AY18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ18">
-        <v>0</v>
-      </c>
-      <c r="BA18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ18" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA18">
+        <v>0</v>
+      </c>
+      <c r="BB18" t="s">
         <v>3</v>
       </c>
-      <c r="BB18" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC18" s="22" t="b">
+      <c r="BC18" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD18" s="22" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX5:AY14 C5:C14 AX16:AY18 C16:C18" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16:C18 AY16:AZ18 C5:C14 AY5:AZ14" xr:uid="{1240F49A-5091-456D-B77A-0673AD56E758}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI5:AI14 AI16:AI18" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ16:AJ18 AJ5:AJ14" xr:uid="{8909875A-86FC-4594-BBAF-A364A5851F3C}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D14 D16:D18" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D18 D5:D14" xr:uid="{EC327A6A-3FD9-4228-86E6-BF4DFCBDFAEB}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3749,17 +4216,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F07677-8B44-417E-B263-203C3A91094A}">
   <dimension ref="A3:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="M5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
@@ -3889,7 +4356,7 @@
         <v>259</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>64</v>
@@ -3927,9 +4394,6 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5">
-        <v>1.2</v>
-      </c>
       <c r="R5">
         <v>1.05</v>
       </c>
@@ -3944,10 +4408,116 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="O6" s="43"/>
+      <c r="A6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2018</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="O7" s="43"/>
+      <c r="A7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>314</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>2018</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="43">
+        <v>0.11</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:21">
       <c r="O8" s="43"/>
@@ -5345,10 +5915,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40:C44 C5:C38 C49:C51" xr:uid="{CE4DB086-8939-4E0F-A217-D1528E507A37}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40:C44 C49:C51 C5:C38" xr:uid="{CE4DB086-8939-4E0F-A217-D1528E507A37}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31:D33 D5:D16 D18:D20 D35:D38 D27:D29 D22:D24 D40:D41 D43:D44 D49:D51" xr:uid="{B6635BCF-58EB-45FF-9851-3E5464D67D97}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31:D33 D49:D51 D18:D20 D35:D38 D27:D29 D22:D24 D40:D41 D43:D44 D5:D16" xr:uid="{B6635BCF-58EB-45FF-9851-3E5464D67D97}">
       <formula1>"singleTier,multiTier"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5709,10 +6279,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C9FDD0-43C0-4547-B8AB-B7BD31607ED6}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5781,7 +6351,7 @@
         <v>5692</v>
       </c>
       <c r="E7" s="85">
-        <f t="shared" ref="E7:E38" si="0">SUM(C7:D7)</f>
+        <f t="shared" ref="E7:E43" si="0">SUM(C7:D7)</f>
         <v>11081</v>
       </c>
     </row>
@@ -6160,76 +6730,159 @@
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="99" t="s">
+        <v>303</v>
+      </c>
+      <c r="C34" s="117">
+        <v>12070</v>
+      </c>
+      <c r="D34" s="114">
+        <v>38475</v>
+      </c>
+      <c r="E34" s="121">
+        <f t="shared" ref="E34" si="6">SUM(C34:D34)</f>
+        <v>50545</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="130" t="s">
+        <v>264</v>
+      </c>
+      <c r="C35" s="137">
+        <f>C29/C$34</f>
+        <v>0.31292460646230325</v>
+      </c>
+      <c r="D35" s="137">
+        <f t="shared" ref="D35:E35" si="7">D29/D$34</f>
+        <v>0.27992202729044835</v>
+      </c>
+      <c r="E35" s="137">
+        <f t="shared" si="7"/>
+        <v>0.28780294786823624</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="130" t="s">
+        <v>265</v>
+      </c>
+      <c r="C36" s="137">
+        <f t="shared" ref="C36:E36" si="8">C30/C$34</f>
+        <v>4.7224523612261803E-3</v>
+      </c>
+      <c r="D36" s="137">
+        <f t="shared" si="8"/>
+        <v>7.3242365172189738E-2</v>
+      </c>
+      <c r="E36" s="137">
+        <f t="shared" si="8"/>
+        <v>5.6880007913740233E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="130" t="s">
+        <v>266</v>
+      </c>
+      <c r="C37" s="137">
+        <f t="shared" ref="C37:E37" si="9">C31/C$34</f>
+        <v>5.0538525269262632E-3</v>
+      </c>
+      <c r="D37" s="137">
+        <f t="shared" si="9"/>
+        <v>4.3664717348927875E-3</v>
+      </c>
+      <c r="E37" s="137">
+        <f t="shared" si="9"/>
+        <v>4.5306162825205264E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="130" t="s">
+        <v>267</v>
+      </c>
+      <c r="C38" s="137">
+        <f t="shared" ref="C38:E38" si="10">C32/C$34</f>
+        <v>0.3203811101905551</v>
+      </c>
+      <c r="D38" s="137">
+        <f t="shared" si="10"/>
+        <v>0.21980506822612086</v>
+      </c>
+      <c r="E38" s="137">
+        <f t="shared" si="10"/>
+        <v>0.24382233653180335</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="74" t="s">
         <v>269</v>
       </c>
-      <c r="C34" s="79">
+      <c r="C39" s="79">
         <v>47</v>
       </c>
-      <c r="D34" s="79">
+      <c r="D39" s="79">
         <v>661</v>
       </c>
-      <c r="E34" s="85">
+      <c r="E39" s="85">
         <f t="shared" si="0"/>
         <v>708</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="75" t="s">
+    <row r="40" spans="2:5">
+      <c r="B40" s="75" t="s">
         <v>279</v>
       </c>
-      <c r="C35" s="88">
+      <c r="C40" s="88">
         <v>7809</v>
       </c>
-      <c r="D35" s="88">
+      <c r="D40" s="88">
         <v>22874</v>
       </c>
-      <c r="E35" s="86">
+      <c r="E40" s="86">
         <f t="shared" si="0"/>
         <v>30683</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="71" t="s">
+    <row r="41" spans="2:5">
+      <c r="B41" s="71" t="s">
         <v>264</v>
       </c>
-      <c r="C36" s="72">
+      <c r="C41" s="72">
         <v>6117</v>
       </c>
-      <c r="D36" s="72">
+      <c r="D41" s="72">
         <v>17854</v>
       </c>
-      <c r="E36" s="85">
+      <c r="E41" s="85">
         <f t="shared" si="0"/>
         <v>23971</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="71" t="s">
+    <row r="42" spans="2:5">
+      <c r="B42" s="71" t="s">
         <v>276</v>
       </c>
-      <c r="C37" s="72">
+      <c r="C42" s="72">
         <v>1692</v>
       </c>
-      <c r="D37" s="72">
+      <c r="D42" s="72">
         <v>5020</v>
       </c>
-      <c r="E37" s="85">
+      <c r="E42" s="85">
         <f t="shared" si="0"/>
         <v>6712</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="77" t="s">
+    <row r="43" spans="2:5">
+      <c r="B43" s="77" t="s">
         <v>280</v>
       </c>
-      <c r="C38" s="78">
+      <c r="C43" s="78">
         <v>1838622</v>
       </c>
-      <c r="D38" s="78">
+      <c r="D43" s="78">
         <v>3149805</v>
       </c>
-      <c r="E38" s="86">
+      <c r="E43" s="86">
         <f t="shared" si="0"/>
         <v>4988427</v>
       </c>
@@ -6245,10 +6898,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9EC4B5-9019-48D6-98E7-5EB690EA862C}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6528,6 +7181,10 @@
       <c r="E24" s="114">
         <v>3813</v>
       </c>
+      <c r="F24" s="121">
+        <f>SUM(D24:E24)</f>
+        <v>5421</v>
+      </c>
     </row>
     <row r="25" spans="3:6">
       <c r="C25" s="99" t="s">
@@ -6539,6 +7196,10 @@
       <c r="E25" s="100">
         <v>2012</v>
       </c>
+      <c r="F25" s="121">
+        <f t="shared" ref="F25:F29" si="5">SUM(D25:E25)</f>
+        <v>2143</v>
+      </c>
     </row>
     <row r="26" spans="3:6">
       <c r="C26" s="99" t="s">
@@ -6550,6 +7211,10 @@
       <c r="E26" s="103">
         <v>121</v>
       </c>
+      <c r="F26" s="121">
+        <f t="shared" si="5"/>
+        <v>168</v>
+      </c>
     </row>
     <row r="27" spans="3:6" ht="25.5">
       <c r="C27" s="99" t="s">
@@ -6561,6 +7226,10 @@
       <c r="E27" s="106">
         <v>4566</v>
       </c>
+      <c r="F27" s="121">
+        <f t="shared" si="5"/>
+        <v>6430</v>
+      </c>
     </row>
     <row r="28" spans="3:6" ht="25.5">
       <c r="C28" s="107" t="s">
@@ -6572,6 +7241,10 @@
       <c r="E28" s="115">
         <v>10513</v>
       </c>
+      <c r="F28" s="121">
+        <f t="shared" si="5"/>
+        <v>14163</v>
+      </c>
     </row>
     <row r="29" spans="3:6">
       <c r="C29" s="108" t="s">
@@ -6583,6 +7256,10 @@
       <c r="E29" s="114">
         <v>38475</v>
       </c>
+      <c r="F29" s="121">
+        <f t="shared" si="5"/>
+        <v>50545</v>
+      </c>
     </row>
     <row r="30" spans="3:6">
       <c r="C30" s="108" t="s">
@@ -6594,26 +7271,98 @@
       <c r="E30" s="109">
         <v>0.2732</v>
       </c>
+      <c r="F30" s="25">
+        <f>F28/F29</f>
+        <v>0.28020575724601837</v>
+      </c>
     </row>
     <row r="31" spans="3:6">
-      <c r="C31" s="99" t="s">
+      <c r="C31" s="135" t="s">
+        <v>302</v>
+      </c>
+      <c r="D31" s="109">
+        <f>D24/D$29</f>
+        <v>0.13322286661143332</v>
+      </c>
+      <c r="E31" s="109">
+        <f>E24/E$29</f>
+        <v>9.9103313840155943E-2</v>
+      </c>
+      <c r="F31" s="109">
+        <f>F24/F$29</f>
+        <v>0.10725096448709071</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="136" t="s">
+        <v>299</v>
+      </c>
+      <c r="D32" s="109">
+        <f t="shared" ref="D32:F32" si="6">D25/D$29</f>
+        <v>1.0853355426677713E-2</v>
+      </c>
+      <c r="E32" s="109">
+        <f t="shared" si="6"/>
+        <v>5.2293697205977908E-2</v>
+      </c>
+      <c r="F32" s="109">
+        <f t="shared" si="6"/>
+        <v>4.2397863290137498E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6">
+      <c r="C33" s="136" t="s">
+        <v>300</v>
+      </c>
+      <c r="D33" s="109">
+        <f t="shared" ref="D33:F33" si="7">D26/D$29</f>
+        <v>3.8939519469759734E-3</v>
+      </c>
+      <c r="E33" s="109">
+        <f t="shared" si="7"/>
+        <v>3.1448992852501625E-3</v>
+      </c>
+      <c r="F33" s="109">
+        <f t="shared" si="7"/>
+        <v>3.3237708972202987E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" s="136" t="s">
+        <v>301</v>
+      </c>
+      <c r="D34" s="109">
+        <f t="shared" ref="D34:F34" si="8">D27/D$29</f>
+        <v>0.1544324772162386</v>
+      </c>
+      <c r="E34" s="109">
+        <f t="shared" si="8"/>
+        <v>0.11867446393762184</v>
+      </c>
+      <c r="F34" s="109">
+        <f t="shared" si="8"/>
+        <v>0.12721337422099119</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6">
+      <c r="C35" s="99" t="s">
         <v>286</v>
       </c>
-      <c r="D31" s="110">
+      <c r="D35" s="110">
         <v>0.2379</v>
       </c>
-      <c r="E31" s="110">
+      <c r="E35" s="110">
         <v>0.21640000000000001</v>
       </c>
     </row>
-    <row r="32" spans="3:6">
-      <c r="C32" s="99" t="s">
+    <row r="36" spans="3:6">
+      <c r="C36" s="99" t="s">
         <v>294</v>
       </c>
-      <c r="D32" s="110">
+      <c r="D36" s="110">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="E32" s="110">
+      <c r="E36" s="110">
         <v>5.6800000000000003E-2</v>
       </c>
     </row>

</xml_diff>